<commit_message>
WIP_variables globales aplicadas con exito como parámetros:totalResults,typeOfPlace, searchTerm
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,7 +466,7 @@
         <v>Web no disponible</v>
       </c>
       <c r="F2" t="str">
-        <v>miércoles, De 09:30 a 19:30, ,jueves, De 09:30 a 19:30, Copiar el horario,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario</v>
+        <v>jueves, De 09:30 a 19:30, ,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario</v>
       </c>
       <c r="G2" t="str">
         <v>Durango</v>
@@ -481,20 +481,19 @@
         <v>4.2</v>
       </c>
       <c r="K2" t="str">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L2" t="str">
         <v>Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad</v>
       </c>
       <c r="M2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                &lt;h2&gt;Vivero Santa Fe&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Blvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 235 9375&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:30 a 19:30, ,jueves, De 09:30 a 19:30, Copiar el horario,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                    
-                </v>
+                    &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
+                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Blvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 235 9375&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:30 a 19:30, ,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
       <c r="N2" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
@@ -520,7 +519,7 @@
         <v>Web no disponible</v>
       </c>
       <c r="F3" t="str">
-        <v>miércoles, De 09:00 a 18:00, ,jueves, De 09:00 a 18:00, Copiar el horario,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario</v>
+        <v>jueves, De 09:00 a 18:00, ,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario</v>
       </c>
       <c r="G3" t="str">
         <v>Durango</v>
@@ -543,13 +542,12 @@
       </c>
       <c r="M3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                &lt;h2&gt;Vivero Las Magnolias&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Sauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 129 7673&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 18:00, ,jueves, De 09:00 a 18:00, Copiar el horario,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                    
-                </v>
+                    &lt;h2&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/h2&gt;
+                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Sauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 129 7673&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 18:00, ,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
       <c r="N3" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
@@ -575,7 +573,7 @@
         <v>https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5</v>
       </c>
       <c r="F4" t="str">
-        <v>miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario</v>
+        <v>jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G4" t="str">
         <v>Durango</v>
@@ -597,13 +595,12 @@
       </c>
       <c r="M4" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                &lt;h2&gt;VIVERO´S AVE DE PARAISO&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Calle Nazas 614, Los Sauces, 34078 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 818 0964&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5"&gt;Web del vivero VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;                    
-                </v>
+                    &lt;h2&gt;Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/h2&gt;
+                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Calle Nazas 614, Los Sauces, 34078 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 818 0964&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5"&gt;Web del vivero VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
       <c r="N4" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no</v>
@@ -629,7 +626,7 @@
         <v>http://macetasvivero.com.mx/directorio-viveros/durango/</v>
       </c>
       <c r="F5" t="str">
-        <v>miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario</v>
+        <v>jueves, De 09:00 a 19:00, ,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G5" t="str">
         <v>Durango</v>
@@ -652,13 +649,12 @@
       </c>
       <c r="M5" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                &lt;h2&gt;Viveros Del Guadiana&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 825 3855&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="http://macetasvivero.com.mx/directorio-viveros/durango/"&gt;Web del vivero Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/data=!4m7!3m6!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1!19sChIJd_X5EgXIm4YRXriokyANA6Q?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;                    
-                </v>
+                    &lt;h2&gt;Parque Ecoturístico Viveros Del Guadiana&lt;/h2&gt;
+                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 825 3855&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 19:00, ,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="http://macetasvivero.com.mx/directorio-viveros/durango/"&gt;Web del vivero Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/data=!4m7!3m6!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1!19sChIJd_X5EgXIm4YRXriokyANA6Q?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
       <c r="N5" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no</v>
@@ -684,7 +680,7 @@
         <v>Web no disponible</v>
       </c>
       <c r="F6" t="str">
-        <v>miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario</v>
+        <v>jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G6" t="str">
         <v>Durango</v>
@@ -708,295 +704,23 @@
       </c>
       <c r="M6" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                &lt;h2&gt;Vivero Santa Fe&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;C. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 120 0604&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                    
-                </v>
+                    &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
+                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;C. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 120 0604&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
       <c r="N6" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no</v>
       </c>
       <c r="O6" t="str">
         <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="7" xml:space="preserve">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Vivero Las Palmas De Veracruz</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Calle Cto. Interior 208, Residencial Santa Teresa, 34166 Durango, Dgo.</v>
-      </c>
-      <c r="D7" t="str">
-        <v>675 113 9208</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="F7" t="str">
-        <v>miércoles, De 09:00 a 20:00, ,jueves, De 09:00 a 20:00, Copiar el horario,viernes, De 09:00 a 20:00, Copiar el horario,sábado, De 09:00 a 20:00, Copiar el horario,domingo, De 09:00 a 16:00, Copiar el horario,lunes, De 09:00 a 20:00, Copiar el horario,martes, De 09:00 a 20:00, Copiar el horario</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H7" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/data=!4m7!3m6!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk!19sChIJZVHDa_i3m4YRsgGC1azTLiw?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I7" t="str">
-        <v>2932+JC Durango</v>
-      </c>
-      <c r="J7" t="str">
-        <v>4.6</v>
-      </c>
-      <c r="K7" t="str">
-        <v>65</v>
-      </c>
-      <c r="L7" t="str">
-        <v>En este vivero hay una gran variedad de plantas, flores 🥀, tierra, árboles etc. A muy buenos precios y una excelente atención lo recomiendo…,Muy amables, la señora que atiende es muy amable, te explica sobre las plantas, sólo que llega mucha gente y la abordan todos juntos, pero ella es muy linda y amable, además de que sus plantas super bonitas y muy cuidaditas.,Buen inventario de plantas y serviciales</v>
-      </c>
-      <c r="M7" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                &lt;h2&gt;Vivero Las Palmas De Veracruz&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Calle Cto. Interior 208, Residencial Santa Teresa, 34166 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;675 113 9208&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 20:00, ,jueves, De 09:00 a 20:00, Copiar el horario,viernes, De 09:00 a 20:00, Copiar el horario,sábado, De 09:00 a 20:00, Copiar el horario,domingo, De 09:00 a 16:00, Copiar el horario,lunes, De 09:00 a 20:00, Copiar el horario,martes, De 09:00 a 20:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Palmas+De+Veracruz/data=!4m7!3m6!1s0x869bb7f86bc35165:0x2c2ed3acd58201b2!8m2!3d24.0040886!4d-104.6488795!16s%2Fg%2F11b6j9p3hk!19sChIJZVHDa_i3m4YRsgGC1azTLiw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Las Palmas De Veracruz&lt;/a&gt;&lt;/p&gt;                    
-                </v>
-      </c>
-      <c r="N7" t="str">
-        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwkGRxLZniTxyzpGYgWgy0om-zTIIXKfSa4Qp54SSDvzr0FdcUHiqajiwFghG4dC8OaeETYzw8f3jUEFSwCI7coOm8Qs1PImZF02qnuYLzrDeUeXbfB4fVM_gpaH6Kwzw6Ilwb0C-1ug1VoBtePqkAVTDOFPRUEgRfDtvr3zKi7nbpfuHMBcQxw_OhGo3jE6L6sUOUM=w408-h726-k-no</v>
-      </c>
-      <c r="O7" t="str">
-        <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="8" xml:space="preserve">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Vivero Santos</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Blvd. Luis Donaldo Colosio M. 109, La Forestal, 34217 Durango, Dgo.</v>
-      </c>
-      <c r="D8" t="str">
-        <v>618 107 2833</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="F8" t="str">
-        <v>miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:00 a 19:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H8" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Santos/data=!4m7!3m6!1s0x869bb7d6349387f9:0x5f5970606c2c7ea8!8m2!3d24.0385842!4d-104.657476!16s%2Fg%2F11b6hvymy7!19sChIJ-YeTNNa3m4YRqH4sbGBwWV8?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I8" t="str">
-        <v>28QV+C2 Durango</v>
-      </c>
-      <c r="J8" t="str">
-        <v>4.6</v>
-      </c>
-      <c r="K8" t="str">
-        <v>15</v>
-      </c>
-      <c r="L8" t="str">
-        <v>Mucho surtido excelente atención.  Bastante ayuda con la asesoría gratuita que me Proporcionaron.  en verdad te ayudan a hacer realidad tu proyecto de remodelación  de jardín.,Es un lugar muy lindo y el sr muy amable llama uno y le da informes,tienen muchas suculentas y cactus a buen precio</v>
-      </c>
-      <c r="M8" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                &lt;h2&gt;Vivero Santos&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Blvd. Luis Donaldo Colosio M. 109, La Forestal, 34217 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 107 2833&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:00 a 19:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santos/data=!4m7!3m6!1s0x869bb7d6349387f9:0x5f5970606c2c7ea8!8m2!3d24.0385842!4d-104.657476!16s%2Fg%2F11b6hvymy7!19sChIJ-YeTNNa3m4YRqH4sbGBwWV8?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Santos&lt;/a&gt;&lt;/p&gt;                    
-                </v>
-      </c>
-      <c r="N8" t="str">
-        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwm26iLtlIwOhXT-d231R-3QlHNTzOeO4QduiUYvULBpbpRE6S5yUI7GsyDjtb39Eg65EtworhXGKy34_voYEdrum8O4zLSgwspg2uLt5Fix_bXC_KPgGHC3LwOjl3aLdlU8ojzIluOAVPvQVsds2XcjeaGHiOR_VhCznQJlTjDzBfMvIM-HvCO4Tfqz3ZTrr8haf9c=w427-h240-k-no</v>
-      </c>
-      <c r="O8" t="str">
-        <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="9" xml:space="preserve">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Vivero Las Nubes</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Av Fidel Velázquez Sánchez, Nuevo Pedregal, Las Nubes, 34224 Durango, Dgo.</v>
-      </c>
-      <c r="D9" t="str">
-        <v>No cuenta con teléfono</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="F9" t="str">
-        <v>miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:30 a 16:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario</v>
-      </c>
-      <c r="G9" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H9" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Las+Nubes/data=!4m7!3m6!1s0x869bb71dcf83f9bb:0x30182ba89df601ac!8m2!3d24.052367!4d-104.595552!16s%2Fg%2F11b6h_sf8h!19sChIJu_mDzx23m4YRrAH2nagrGDA?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I9" t="str">
-        <v>3C23+WQ Durango</v>
-      </c>
-      <c r="J9" t="str">
-        <v>4.4</v>
-      </c>
-      <c r="K9" t="str">
-        <v>117</v>
-      </c>
-      <c r="L9" t="str">
-        <v>Gran vivero con muchas opciones hermosas de plantas a un buen precio, trato muy amable. Abren los domingos y eso también es una gran ventaja ya que es cuando mucha gente tiene tiempo libre y busca opciones para decorar su hogar. ¡Recomendado!,Siempre tiene plantas muy bonitas. Más el viernes en la tarde, excelente trato y te dan tips,Tienen una excelente variedad de plantas y el señor que atendió sabe mucho de plantas.</v>
-      </c>
-      <c r="M9" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                &lt;h2&gt;Vivero Las Nubes&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Av Fidel Velázquez Sánchez, Nuevo Pedregal, Las Nubes, 34224 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;No cuenta con teléfono&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:30 a 16:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Nubes/data=!4m7!3m6!1s0x869bb71dcf83f9bb:0x30182ba89df601ac!8m2!3d24.052367!4d-104.595552!16s%2Fg%2F11b6h_sf8h!19sChIJu_mDzx23m4YRrAH2nagrGDA?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Las Nubes&lt;/a&gt;&lt;/p&gt;                    
-                </v>
-      </c>
-      <c r="N9" t="str">
-        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwnxvkXJNc_oGxVqBb7qfpz6zUdmPmSJ7SHu0dl5jQByhqaJuy5Xr2HUzWRML1leuuo4ExFFgGpJxzTTlYDtCPX_kZW_PJgOb0fO9-imalYNPQRdVm-ngtKdh9-QrYJAciR1ky5MoVPdcgscTTbWn5hoQcEsH5YJuus7LIfQ10h9J9vfbl53AY6IEDAr1PF1SCe7vQ=w408-h726-k-no</v>
-      </c>
-      <c r="O9" t="str">
-        <v>Añadir número de teléfono del sitio,Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="10" xml:space="preserve">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Vivero El Milagro Suc Los Angeles</v>
-      </c>
-      <c r="C10" t="str">
-        <v>C. Aquiles Serdan 1306, Los Ángeles, 34076 Durango, Dgo.</v>
-      </c>
-      <c r="D10" t="str">
-        <v>618 189 0754</v>
-      </c>
-      <c r="E10" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="F10" t="str">
-        <v>miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 23:00, Copiar el horario,domingo, De 08:00 a 23:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario</v>
-      </c>
-      <c r="G10" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H10" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+El+Milagro+Suc+Los+Angeles/data=!4m7!3m6!1s0x869bc83f03010ed1:0x1db0e10487ed912!8m2!3d24.0267101!4d-104.6794677!16s%2Fg%2F11b6j6cy2v!19sChIJ0Q4BAz_Im4YREtl-SBAO2wE?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I10" t="str">
-        <v>28GC+M6 Durango</v>
-      </c>
-      <c r="J10" t="str">
-        <v>4.2</v>
-      </c>
-      <c r="K10" t="str">
-        <v>11</v>
-      </c>
-      <c r="L10" t="str" xml:space="preserve">
-        <v xml:space="preserve">Muy bonito lugar, precios moderados,  buenas bebidas y snacks,La comida estuvo buena.
-El servicio a cliente es pésimo, las chicas son muy groseras e incómodan con su actitud. Problemas al tomar la orden.,Hay muy poca variedad de maceta floral</v>
-      </c>
-      <c r="M10" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                &lt;h2&gt;Vivero El Milagro Suc Los Angeles&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;C. Aquiles Serdan 1306, Los Ángeles, 34076 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;618 189 0754&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 08:00 a 19:00, ,jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 23:00, Copiar el horario,domingo, De 08:00 a 23:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+El+Milagro+Suc+Los+Angeles/data=!4m7!3m6!1s0x869bc83f03010ed1:0x1db0e10487ed912!8m2!3d24.0267101!4d-104.6794677!16s%2Fg%2F11b6j6cy2v!19sChIJ0Q4BAz_Im4YREtl-SBAO2wE?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero El Milagro Suc Los Angeles&lt;/a&gt;&lt;/p&gt;                    
-                </v>
-      </c>
-      <c r="N10" t="str">
-        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwk6RTo_YEdEOr09MT5Ei_cOtZNqhQ0OqTu29yUeBFVH3PEn7Ge8Tcav4EUPsckeMP6PvnbIiMRNVlcQwidTCLFVpBPB7SIoFbhxaTkaEa9f0SmcscPO81faSCyuvaF1w7MHWQzeCTMclJzCp5zKmDmr7oyVW3uTiBe1VHxz5y3iM1FKMjdMdg5SsovcGNtoUlDW3g=w427-h240-k-no</v>
-      </c>
-      <c r="O10" t="str">
-        <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="11" xml:space="preserve">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Vivero Victoria</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Av. del Factor 906, Casa Redonda, 35158 Durango, Dgo.</v>
-      </c>
-      <c r="D11" t="str">
-        <v>No cuenta con teléfono</v>
-      </c>
-      <c r="E11" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="F11" t="str">
-        <v>miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:00 a 19:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario</v>
-      </c>
-      <c r="G11" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H11" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Victoria/data=!4m7!3m6!1s0x869bc82f1e35ef4b:0x28ac0bb71cd10463!8m2!3d24.0391699!4d-104.6661015!16s%2Fg%2F11b6j5hybg!19sChIJS-81Hi_Im4YRYwTRHLcLrCg?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I11" t="str">
-        <v>28QM+MH Durango</v>
-      </c>
-      <c r="J11" t="str">
-        <v>4.3</v>
-      </c>
-      <c r="K11" t="str">
-        <v>7</v>
-      </c>
-      <c r="L11" t="str">
-        <v>Cuando fui no sabían que veriedad eran los árboles, aún que tenían de muchos tipos, los dan muy económicos.,Mucha variedad de plantas,Buen servicio</v>
-      </c>
-      <c r="M11" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                &lt;h2&gt;Vivero Victoria&lt;/h2&gt;
-                &lt;p&gt;&lt;b&gt;Dirección del vivero: &lt;/b&gt;Av. del Factor 906, Casa Redonda, 35158 Durango, Dgo.&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Teléfono: &lt;/b&gt;No cuenta con teléfono&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Horarios: &lt;/b&gt;miércoles, De 09:00 a 19:00, ,jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 19:00, Copiar el horario,domingo, De 09:00 a 19:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Victoria/data=!4m7!3m6!1s0x869bc82f1e35ef4b:0x28ac0bb71cd10463!8m2!3d24.0391699!4d-104.6661015!16s%2Fg%2F11b6j5hybg!19sChIJS-81Hi_Im4YRYwTRHLcLrCg?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del vivero Vivero Victoria&lt;/a&gt;&lt;/p&gt;                    
-                </v>
-      </c>
-      <c r="N11" t="str">
-        <v>https://lh3.googleusercontent.com/gps-proxy/ALm4wwn5g1i4E_QGBMFVZBTMDOPFqfR45RgpPMuLVjFL1Vg5W8Pzf2COZzhV2HmEETpdewFUvPEIczoLt87fgVeCvJbYAOE4edEvOB4lYlytp2_2jxUbh8IZuHKNUV8_xLewDZBMWrSUxTSeXYRtTn---5GjEtNyvBBn3vdLCx7p2xiRdCFj16JJE1HA_LXKut19aonzDqY=w427-h240-k-no</v>
-      </c>
-      <c r="O11" t="str">
-        <v>Añadir número de teléfono del sitio,Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_Descifrando limpieza de arrayHorario en archivo functions.js
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -465,9 +465,6 @@
       <c r="E2" t="str">
         <v>Web no disponible</v>
       </c>
-      <c r="F2" t="str">
-        <v>jueves, De 09:30 a 19:30, ,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario</v>
-      </c>
       <c r="G2" t="str">
         <v>Durango</v>
       </c>
@@ -491,7 +488,7 @@
                     &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Blvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 235 9375&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:30 a 19:30, ,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:30 a 19:30, Copiar el horario,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -517,9 +514,6 @@
       </c>
       <c r="E3" t="str">
         <v>Web no disponible</v>
-      </c>
-      <c r="F3" t="str">
-        <v>jueves, De 09:00 a 18:00, ,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario</v>
       </c>
       <c r="G3" t="str">
         <v>Durango</v>
@@ -545,7 +539,7 @@
                     &lt;h2&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Sauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 129 7673&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 18:00, ,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 18:00, Copiar el horario,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -571,9 +565,6 @@
       </c>
       <c r="E4" t="str">
         <v>https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5</v>
-      </c>
-      <c r="F4" t="str">
-        <v>jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G4" t="str">
         <v>Durango</v>
@@ -598,7 +589,7 @@
                     &lt;h2&gt;Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Calle Nazas 614, Los Sauces, 34078 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 818 0964&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5"&gt;Web del vivero VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -624,9 +615,6 @@
       </c>
       <c r="E5" t="str">
         <v>http://macetasvivero.com.mx/directorio-viveros/durango/</v>
-      </c>
-      <c r="F5" t="str">
-        <v>jueves, De 09:00 a 19:00, ,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G5" t="str">
         <v>Durango</v>
@@ -652,7 +640,7 @@
                     &lt;h2&gt;Parque Ecoturístico Viveros Del Guadiana&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 825 3855&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 19:00, ,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="http://macetasvivero.com.mx/directorio-viveros/durango/"&gt;Web del vivero Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/data=!4m7!3m6!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1!19sChIJd_X5EgXIm4YRXriokyANA6Q?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -678,9 +666,6 @@
       </c>
       <c r="E6" t="str">
         <v>Web no disponible</v>
-      </c>
-      <c r="F6" t="str">
-        <v>jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario</v>
       </c>
       <c r="G6" t="str">
         <v>Durango</v>
@@ -707,7 +692,7 @@
                     &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;C. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 120 0604&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, ,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>

</xml_diff>

<commit_message>
WIP_Implementando limpieza de arrayHorario en archivo googleMaps.js
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -488,7 +488,7 @@
                     &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Blvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 235 9375&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:30 a 19:30, Copiar el horario,viernes, De 09:30 a 19:30, Copiar el horario,sábado, De 09:30 a 19:30, Copiar el horario,domingo, De 09:30 a 19:30, Copiar el horario,lunes, De 09:30 a 19:30, Copiar el horario,martes, De 09:30 a 19:30, Copiar el horario,miércoles, De 09:30 a 19:30, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -539,7 +539,7 @@
                     &lt;h2&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/h2&gt;
                     &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Sauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 129 7673&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 18:00, Copiar el horario,viernes, De 09:00 a 18:00, Copiar el horario,sábado, De 09:00 a 18:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 09:00 a 18:00, Copiar el horario,martes, De 09:00 a 18:00, Copiar el horario,miércoles, De 09:00 a 18:00, Copiar el horario&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        </v>
       </c>
@@ -547,165 +547,12 @@
         <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
       </c>
       <c r="O3" t="str">
-        <v>Añadir sitio web</v>
-      </c>
-    </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>VIVERO´S AVE DE PARAISO</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Calle Nazas 614, Los Sauces, 34078 Durango, Dgo.</v>
-      </c>
-      <c r="D4" t="str">
-        <v>618 818 0964</v>
-      </c>
-      <c r="E4" t="str">
-        <v>https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H4" t="str">
-        <v>https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I4" t="str">
-        <v>2954+C6 Durango</v>
-      </c>
-      <c r="J4" t="str">
-        <v>4.3</v>
-      </c>
-      <c r="K4" t="str">
-        <v>21</v>
-      </c>
-      <c r="L4" t="str">
-        <v>Mala atención,Las nochebuenas estan hermosas, no me fui de ahí sin las mías, lastimas que el resto de plantas están muy amontonadas y no se pueden apreciar bien,Tienen una gran variedad de plantas</v>
-      </c>
-      <c r="M4" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/h2&gt;
-                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Calle Nazas 614, Los Sauces, 34078 Durango, Dgo.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 818 0964&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 17:00, Copiar el horario,domingo, De 09:00 a 17:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="https://www.instagram.com/invites/contact/?i=1rjinh0zovkbr&amp;utm_content=myh4mm5"&gt;Web del vivero VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/VIVERO%C2%B4S+AVE+DE+PARAISO/data=!4m7!3m6!1s0x869bb7f0d4ea30ef:0x4cb36ed930d8acad!8m2!3d24.008504!4d-104.644488!16s%2Fg%2F11ddx2_b8h!19sChIJ7zDq1PC3m4YRrazYMNlus0w?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico VIVERO´S AVE DE PARAISO&lt;/a&gt;&lt;/p&gt;                        </v>
-      </c>
-      <c r="N4" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipMOYk2QlPDlj4I6VmQIIolnA3Ipl8mWjdIXSvrS=w408-h725-k-no</v>
-      </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Viveros Del Guadiana</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.</v>
-      </c>
-      <c r="D5" t="str">
-        <v>618 825 3855</v>
-      </c>
-      <c r="E5" t="str">
-        <v>http://macetasvivero.com.mx/directorio-viveros/durango/</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H5" t="str">
-        <v>https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/data=!4m7!3m6!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1!19sChIJd_X5EgXIm4YRXriokyANA6Q?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I5" t="str">
-        <v>286J+6G Durango</v>
-      </c>
-      <c r="J5" t="str">
-        <v>5.0</v>
-      </c>
-      <c r="K5" t="str">
-        <v>4</v>
-      </c>
-      <c r="L5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Bastante variedad de plantas, se adaptan en cada temporada del año, ahora para fiestas de navideñas cuentan con variedad de noche buenas, además que también ofrecen el servicio de diseño y mantenimiento para jardines.…,Me gustó este lugar, tiene variedad de plantas 🌱 ahí encontré dos gardenias hermosas que ya florecieron y huelen muy bonito. La atención es excelente. Volveré por más plantas 🌹🌸
-🌱🌱…,Gran variedad de plantas y excelente atención.</v>
-      </c>
-      <c r="M5" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;Parque Ecoturístico Viveros Del Guadiana&lt;/h2&gt;
-                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Abasolo 609, Francisco González de la Vega, 34157 Durango, Dgo.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 825 3855&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 09:00 a 19:00, Copiar el horario,viernes, De 09:00 a 19:00, Copiar el horario,sábado, De 09:00 a 17:00, Copiar el horario,domingo, De 10:00 a 15:00, Copiar el horario,lunes, De 09:00 a 19:00, Copiar el horario,martes, De 09:00 a 19:00, Copiar el horario,miércoles, De 09:00 a 19:00, Copiar el horario&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;&lt;a href="http://macetasvivero.com.mx/directorio-viveros/durango/"&gt;Web del vivero Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Viveros+Del+Guadiana/data=!4m7!3m6!1s0x869bc80512f9f577:0xa4030d2093a8b85e!8m2!3d24.0106133!4d-104.6687241!16s%2Fg%2F11b6jd0vv1!19sChIJd_X5EgXIm4YRXriokyANA6Q?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Viveros Del Guadiana&lt;/a&gt;&lt;/p&gt;                        </v>
-      </c>
-      <c r="N5" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipMrQ-GksQ-38r7UjiSPgRrkAk_jvI98IIqdsliq=w426-h240-k-no</v>
-      </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6" xml:space="preserve">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Vivero Santa Fe</v>
-      </c>
-      <c r="C6" t="str">
-        <v>C. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.</v>
-      </c>
-      <c r="D6" t="str">
-        <v>618 120 0604</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Web no disponible</v>
-      </c>
-      <c r="G6" t="str">
-        <v>Durango</v>
-      </c>
-      <c r="H6" t="str">
-        <v>https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>X8V7+FM Durango</v>
-      </c>
-      <c r="J6" t="str">
-        <v>4.4</v>
-      </c>
-      <c r="K6" t="str">
-        <v>52</v>
-      </c>
-      <c r="L6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Gran surtido de plantas y pasto de muy buena calidad,Tiene gran variedad de plantas, pero sus precios no son nada asequibles, inclusive precios triplicados en cuanto a precios en otros viveros...,Muchas plantas muy bonitas
-Para Sol y sombra y buenos precios
-Sí lo recomiendo.</v>
-      </c>
-      <c r="M6" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
-                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;C. Victoria 106, Arroyo Seco, 34147 Durango, Dgo.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 120 0604&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;jueves, De 08:00 a 19:00, Copiar el horario,viernes, De 08:00 a 19:00, Copiar el horario,sábado, De 08:00 a 19:00, Copiar el horario,domingo, De 08:00 a 16:00, Copiar el horario,lunes, De 08:00 a 19:00, Copiar el horario,martes, De 08:00 a 19:00, Copiar el horario,miércoles, De 08:00 a 19:00, Copiar el horario&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bc7de9a5a690f:0x1c9d03d9335b8bbd!8m2!3d23.9936822!4d-104.6858595!16s%2Fg%2F11b6jgmr3h!19sChIJD2lamt7Hm4YRvYtbM9kDnRw?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
-      </c>
-      <c r="N6" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipNrN9F6dstJ2M3M7lFIyGQEZFWkNlnH0euKP8Hi=w426-h240-k-no</v>
-      </c>
-      <c r="O6" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_Creacion del textSpinner, y primeras pruebas de implementación
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -486,7 +486,12 @@
       <c r="M2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
-                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Blvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y conoce los mejores  Parque Ecoturístico de Tabasco!&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;Dirección del Parque Ecoturístico Vivero Santa Fe: &lt;/b&gt;&lt;/h3&gt;
+                    &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 235 9375&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
@@ -537,7 +542,12 @@
       <c r="M3" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/h2&gt;
-                    &lt;p&gt;&lt;b&gt;Dirección del Parque Ecoturístico: &lt;/b&gt;Sauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y conoce los mejores  Parque de Ecoturismo de Tabasco!&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;Dirección del Parque Ecoturístico Vivero Las Magnolias: &lt;/b&gt;&lt;/h3&gt;
+                    &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 129 7673&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;

</xml_diff>

<commit_message>
WIP_textSpinner_Implementación exitosa en el objeto de structuredData(blogPost)
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -485,17 +485,30 @@
       </c>
       <c r="M2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;Parque Ecoturístico Vivero Santa Fe&lt;/h2&gt;
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y conoce los mejores  Parque Ecoturístico de Tabasco!&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;Dirección del Parque Ecoturístico Vivero Santa Fe: &lt;/b&gt;&lt;/h3&gt;
-                    &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 235 9375&lt;/p&gt;
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
+                      &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.2 estrellas de más de Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para ir a este centro manejando, puedes usar esta dirección oficial con tu google maps o usando este  &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los contactos disponibles del Parque Natural Vivero Santa Fe son: &lt;/p&gt;
+                        &lt;ul&gt;
+                            &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
+                            &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
+                        &lt;/ul&gt;
+                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/li&gt;
+                            &lt;/ul&gt;
+                        &lt;p&gt;Siempre es importante -aún si cuentas con estos horarios oficiales-, revisar en sus redes sociales y medios de contacto antes de ir. Así podrás asegurarte de que no hayan tenido ningún cambio de horario o logístico de último momento.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        </v>
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        
+                    </v>
       </c>
       <c r="N2" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
@@ -530,10 +543,10 @@
         <v>29P7+XW Durango</v>
       </c>
       <c r="J3" t="str">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
       <c r="K3" t="str">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L3" t="str" xml:space="preserve">
         <v xml:space="preserve">Excelente atención del joven y mucha variedad de plantas!!
@@ -541,17 +554,30 @@
       </c>
       <c r="M3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;h2&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/h2&gt;
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
  Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y conoce los mejores  Parque de Ecoturismo de Tabasco!&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;Dirección del Parque Ecoturístico Vivero Las Magnolias: &lt;/b&gt;&lt;/h3&gt;
-                    &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Teléfono del Parque Ecoturístico: &lt;/b&gt;618 129 7673&lt;/p&gt;
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
+                    &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
+                      &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.7 respaldada por más de 106visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;El Centro Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para ir a este lugar usar esa dirección en un gps o ayudarte con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Vivero Las Magnolias son: &lt;/p&gt;
+                        &lt;ul&gt;
+                            &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
+                            &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
+                        &lt;/ul&gt;
+                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los horarios oficiales del Centro Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/li&gt;
+                            &lt;/ul&gt;
+                        &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        </v>
+                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        
+                    </v>
       </c>
       <c r="N3" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>

</xml_diff>

<commit_message>
WIP_intentando traducir arrayHorario en arrayObjeto, aún WIP
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -465,6 +465,9 @@
       <c r="E2" t="str">
         <v>Web no disponible</v>
       </c>
+      <c r="F2" t="str">
+        <v>[object Object]</v>
+      </c>
       <c r="G2" t="str">
         <v>Durango</v>
       </c>
@@ -486,26 +489,26 @@
       <c r="M2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
  Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
-                      &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.2 estrellas de más de Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                      &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.2 respaldada por más de 33visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
                     &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para ir a este centro manejando, puedes usar esta dirección oficial con tu google maps o usando este  &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los contactos disponibles del Parque Natural Vivero Santa Fe son: &lt;/p&gt;
+                        &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para ir a este parque, simplemente basta con colocar la dirección en una app de navegación o siguiendo este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
                         &lt;ul&gt;
                             &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
                             &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
                         &lt;/ul&gt;
                     &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;
+                        &lt;p&gt;Los horarios oficiales del Parque de Ecoturismo Vivero Santa Fe son los siguientes:&lt;/p&gt;
                             &lt;ul&gt;
-                                &lt;li&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/li&gt;
+                                &lt;li&gt;[object Object]&lt;/li&gt;
                             &lt;/ul&gt;
-                        &lt;p&gt;Siempre es importante -aún si cuentas con estos horarios oficiales-, revisar en sus redes sociales y medios de contacto antes de ir. Así podrás asegurarte de que no hayan tenido ningún cambio de horario o logístico de último momento.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:30 a 19:30,Sábado de 09:30 a 19:30,Domingo de 09:30 a 19:30,Lunes de 09:30 a 19:30,Martes de 09:30 a 19:30,Miércoles de 09:30 a 19:30,Jueves de 09:30 a 19:30&lt;/p&gt;
+                        &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;[object Object]&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        
                     </v>
@@ -533,6 +536,9 @@
       <c r="E3" t="str">
         <v>Web no disponible</v>
       </c>
+      <c r="F3" t="str">
+        <v>[object Object]</v>
+      </c>
       <c r="G3" t="str">
         <v>Durango</v>
       </c>
@@ -554,27 +560,28 @@
       </c>
       <c r="M3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Natural que han sido mejor evaluados en este estado. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
  Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
-                      &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.7 respaldada por más de 106visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;El Centro Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para ir a este lugar usar esa dirección en un gps o ayudarte con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los contactos disponibles del Parque de Ecoturismo Vivero Las Magnolias son: &lt;/p&gt;
+                      &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.7 estrellas de más de Excelente atención del joven y mucha variedad de plantas!!
+Compré tierra para macetas, me dijo el joven que era muy buena, pero huele muy mal, me pueden dar alguna sugerencia para eliminar ese olor tan fuerte?! Por favor!!,Me encantan todas las plantas, son muy amables, los precios justos🤩…,Muy bonito vivero visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para ir a este sitio, coloca esta dirección en una herramienta de navegación o apóyate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Vivero Las Magnolias son: &lt;/p&gt;
                         &lt;ul&gt;
                             &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
                             &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
                         &lt;/ul&gt;
-                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los horarios oficiales del Centro Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;
+                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;p&gt;Los horarios oficiales del Parque de Ecoturismo Vivero Las Magnolias son los siguientes:&lt;/p&gt;
                             &lt;ul&gt;
-                                &lt;li&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/li&gt;
+                                &lt;li&gt;[object Object]&lt;/li&gt;
                             &lt;/ul&gt;
-                        &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;Viernes de 09:00 a 18:00,Sábado de 09:00 a 18:00,Domingo de 09:00 a 17:00,Lunes de 09:00 a 18:00,Martes de 09:00 a 18:00,Miércoles de 09:00 a 18:00,Jueves de 09:00 a 18:00&lt;/p&gt;
+                        &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;
+                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;[object Object]&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
                     &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        
                     </v>

</xml_diff>

<commit_message>
WIP_arreglando bug por borrado sinquerer de la definición de web en objetoInfo_Completed:)
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -440,12 +440,18 @@
         <v>opiniones</v>
       </c>
       <c r="M1" t="str">
+        <v>photo</v>
+      </c>
+      <c r="N1" t="str">
+        <v>articleIntro</v>
+      </c>
+      <c r="O1" t="str">
         <v>structuredData</v>
       </c>
-      <c r="N1" t="str">
-        <v>photo</v>
-      </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
+        <v>photoLocal</v>
+      </c>
+      <c r="Q1" t="str">
         <v>missingData</v>
       </c>
     </row>
@@ -483,24 +489,31 @@
       <c r="L2" t="str">
         <v>Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad</v>
       </c>
-      <c r="M2" t="str" xml:space="preserve">
+      <c r="M2" t="str">
+        <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
+      </c>
+      <c r="N2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque de Ecoturismo que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Sitio Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="O2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
-                      &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.2 estrellas de más de Super mala atención. Tienen muy bonitas plantas pero la señora que atendie, nunca me hizo caso, le mostre la planta que quería y me ignoro por completo, pésimo. No lo recomiendo y no vuelvo a ir,Excelente atención variedad de plantas  adornos para jardín lo recomiendo Buen Trato y novedades,Excelente atención y plantas de muy buena calidad visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;El Sitio Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
-                        &lt;ul&gt;
-                            &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
-                            &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
-                        &lt;/ul&gt;
-                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Natural Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;
+                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.2 respaldada por más de 33visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Sitio Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:30 a 19:30&lt;/li&gt;
@@ -510,16 +523,15 @@
                                 &lt;li&gt;Sábado de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:30 a 19:30&lt;/li&gt;
                             &lt;/ul&gt;
-                        &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;[object Object]&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;                        
+                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
                     </v>
       </c>
-      <c r="N2" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
-      </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no" alt="Vivero Santa Fe"&gt;                
+                </v>
+      </c>
+      <c r="Q2" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -558,24 +570,31 @@
         <v xml:space="preserve">Excelente atención del joven y mucha variedad de plantas!!
 Compré tierra para macetas, me dijo el joven que era muy buena, pero huele muy mal, me pueden dar alguna sugerencia para eliminar ese olor tan fuerte?! Por favor!!,Me encantan todas las plantas, son muy amables, los precios justos🤩…,Muy bonito vivero</v>
       </c>
-      <c r="M3" t="str" xml:space="preserve">
+      <c r="M3" t="str">
+        <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
+      </c>
+      <c r="N3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Centro Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecológico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
- Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="O3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
-                      &lt;p&gt;Este Parque Ecoturístico tiene 4.7 de calificación promedio, a partir de las más de 106 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;El Parque Natural se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. LLegar al lugar es bastante sencillo. Símplemente coloca la dirección en una app con gps, o apóyate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
-                    &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Natural Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los contactos disponibles del Sitio Ecoturístico Vivero Las Magnolias son: &lt;/p&gt;
-                        &lt;ul&gt;
-                            &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
-                            &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;
-                        &lt;/ul&gt;
-                    &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro de Ecoturismo Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                        &lt;p&gt;Los horarios oficiales del Parque Natural Vivero Las Magnolias son los siguientes:&lt;/p&gt;
+                        &lt;p&gt;Este Parque Ecoturístico tiene 4.7 de calificación promedio, a partir de las más de 106 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecológico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque de Ecoturismo se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para llegar, puedes símplemente colocar esta dirección en el googleMaps o Waze o apoyarte en este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Vivero Las Magnolias son: &lt;/p&gt;
+                            &lt;ul&gt;
+                                &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
+                                &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
+                            &lt;/ul&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecológico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:00 a 18:00&lt;/li&gt;
@@ -585,22 +604,21 @@
                                 &lt;li&gt;Sábado de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 17:00&lt;/li&gt;
                             &lt;/ul&gt;
-                        &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Horarios Oficiales: &lt;/b&gt;[object Object]&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Sitio Web: &lt;/b&gt;web no disponible&lt;/p&gt;
-                    &lt;p&gt;&lt;b&gt;Ubicación: &lt;/b&gt;&lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;                        
+                            &lt;p&gt;Siempre es importante -aún si cuentas con estos horarios oficiales-, revisar en sus redes sociales y medios de contacto antes de ir. Así podrás asegurarte de que no hayan tenido ningún cambio de horario o logístico de último momento.&lt;/p&gt;                 
                     </v>
       </c>
-      <c r="N3" t="str">
-        <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
-      </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no" alt="Vivero Las Magnolias"&gt;                
+                </v>
+      </c>
+      <c r="Q3" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_arreglando método para descarga, manipulación,rename y upload fotografías
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -440,18 +440,33 @@
         <v>opiniones</v>
       </c>
       <c r="M1" t="str">
-        <v>photo</v>
+        <v>photoOriginalURL</v>
       </c>
       <c r="N1" t="str">
+        <v>photoFileName</v>
+      </c>
+      <c r="O1" t="str">
+        <v>photoNewName</v>
+      </c>
+      <c r="P1" t="str">
+        <v>photoNewURL</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>fileNameConversionScript</v>
+      </c>
+      <c r="R1" t="str">
         <v>articleIntro</v>
       </c>
-      <c r="O1" t="str">
+      <c r="S1" t="str">
+        <v>photoNewFileNameFull</v>
+      </c>
+      <c r="T1" t="str">
         <v>structuredData</v>
       </c>
-      <c r="P1" t="str">
+      <c r="U1" t="str">
         <v>photoLocal</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="V1" t="str">
         <v>missingData</v>
       </c>
     </row>
@@ -492,22 +507,42 @@
       <c r="M2" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
       </c>
-      <c r="N2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Sitio Ecoturístico que han sido mejor evaluados en este estado. 
+      <c r="N2" t="str">
+        <v>AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no</v>
+      </c>
+      <c r="O2" t="str">
+        <v>Vivero_Santa_Fe</v>
+      </c>
+      <c r="P2" t="str">
+        <v>https://rumbonaturaleza.com/uploads/2023/03/Vivero_Santa_Fe.jpg</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>ren "AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no" "Vivero_Santa_Fe.jpg"</v>
+      </c>
+      <c r="R2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
  Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
-      <c r="O2" t="str" xml:space="preserve">
+      <c r="S2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="T2" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
                         &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.2 respaldada por más de 33visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Sitio Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para ir a este parque, simplemente basta con colocar la dirección en una app de navegación o siguiendo este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque de Ecoturismo Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Centro de Ecoturismo Vivero Santa Fe son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
@@ -526,12 +561,12 @@
                             &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
                     </v>
       </c>
-      <c r="P2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://lh5.googleusercontent.com/p/AF1QipOC7w7iQu2kg7BiEaF1hoYdzwUX11Mfy6wYJIgK=w408-h306-k-no" alt="Vivero Santa Fe"&gt;                
+      <c r="U2" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="undefined" alt="Vivero Santa Fe"&gt;                
                 </v>
       </c>
-      <c r="Q2" t="str">
+      <c r="V2" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
@@ -573,28 +608,48 @@
       <c r="M3" t="str">
         <v>https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
       </c>
-      <c r="N3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Centro Ecoturístico que han sido mejor evaluados en este estado. 
+      <c r="N3" t="str">
+        <v>AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no</v>
+      </c>
+      <c r="O3" t="str">
+        <v>Vivero_Las_Magnolias</v>
+      </c>
+      <c r="P3" t="str">
+        <v>https://rumbonaturaleza.com/uploads/2023/03/Vivero_Las_Magnolias.jpg</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>ren "AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no" "Vivero_Las_Magnolias.jpg"</v>
+      </c>
+      <c r="R3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
  Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
-      <c r="O3" t="str" xml:space="preserve">
+      <c r="S3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
+                    </v>
+      </c>
+      <c r="T3" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;Este Parque Ecoturístico tiene 4.7 de calificación promedio, a partir de las más de 106 opiniones de sus visitantes... ¿nada mal no?. Es por eso que es parte de esta lista de los Parque Ecoturístico mejor calificados de Tabasco. Con este respaldo estamos más que seguras(os) que se trata  de un sitio que vas a disfrutar al Máximo. Así que ya sabes, si lo que buscas es naturaleza, el Parque Ecoturístico undefineden Tabasco, es sin duda una gran opción&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecológico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque de Ecoturismo se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para llegar, puedes símplemente colocar esta dirección en el googleMaps o Waze o apoyarte en este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro Ecoturístico Vivero Las Magnolias son: &lt;/p&gt;
+                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.7 respaldada por más de 106visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Ecológico Vivero Las Magnolias son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
                         &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del Parque Ecológico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
+                            &lt;p&gt;Los horarios oficiales del Centro Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:00 a 18:00&lt;/li&gt;
@@ -604,21 +659,21 @@
                                 &lt;li&gt;Sábado de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 17:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Siempre es importante -aún si cuentas con estos horarios oficiales-, revisar en sus redes sociales y medios de contacto antes de ir. Así podrás asegurarte de que no hayan tenido ningún cambio de horario o logístico de último momento.&lt;/p&gt;                 
+                            &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;                 
                     </v>
       </c>
-      <c r="P3" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-                    &lt;img src="https://lh5.googleusercontent.com/p/AF1QipPmQSXM5PoyrFj8IU2GdEEKh9C_3Ku5CJxKUUUM=w408-h306-k-no" alt="Vivero Las Magnolias"&gt;                
+      <c r="U3" t="str" xml:space="preserve">
+        <v xml:space="preserve">
+                    &lt;img src="undefined" alt="Vivero Las Magnolias"&gt;                
                 </v>
       </c>
-      <c r="Q3" t="str">
+      <c r="V3" t="str">
         <v>Añadir sitio web</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:V3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP_método para descarga y uso de fotos competado_Completed :)
</commit_message>
<xml_diff>
--- a/viverosDurango.xlsx
+++ b/viverosDurango.xlsx
@@ -521,17 +521,17 @@
       </c>
       <c r="R2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
  Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="S2" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
  Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Parque Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+ Con esta prueba social como respaldo, hoy te daremos los Parque de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
@@ -539,15 +539,15 @@
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Santa Fe&lt;/b&gt;&lt;/h2&gt;
                         &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.2 respaldada por más de 33visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Centro Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para ir a este parque, simplemente basta con colocar la dirección en una app de navegación o siguiendo este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque de Ecoturismo Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Centro de Ecoturismo Vivero Santa Fe son: &lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Ecoturístico Vivero Santa Fe? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Sitio Ecoturístico se ubica enBlvd. Cnel. Enrique Carrola Antuna 909, Ciénega, 34090 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Santa+Fe/data=!4m7!3m6!1s0x869bb7e17f5ebdfd:0x329bbfbf57717ca0!8m2!3d24.0199748!4d-104.6558555!16s%2Fg%2F11btmr25_0!19sChIJ_b1ef-G3m4YRoHxxV7-_mzI?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Santa Fe&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecológico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Ecoturístico Vivero Santa Fe son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 235 9375&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Centro Ecoturístico Vivero Santa Fe?&lt;/b&gt;&lt;/h3&gt;
                             &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Santa Fe son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 09:30 a 19:30&lt;/li&gt;
@@ -558,7 +558,7 @@
                                 &lt;li&gt;Sábado de 09:30 a 19:30&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:30 a 19:30&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Aunque cuentes ya con los horarios oficiales de apertura de este lugar, siempre te recomendamos que antes de ir eches un ojito a sus redes sociales y vías de contacto, para asegurarte de que no hayan tenido algún cambio logístico de última hora&lt;/p&gt;                 
+                            &lt;p&gt;Aunque estos horarios sean oficialmente vigentes, nunca está de más que antes de lanzarte, revises en sus redes sociales o contactos digitales que no haya habido ningún cambio logístico extraordinario en sus horarios de apertura y cierre.&lt;/p&gt;                 
                     </v>
       </c>
       <c r="U2" t="str" xml:space="preserve">
@@ -622,34 +622,35 @@
       </c>
       <c r="R3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="S3" t="str" xml:space="preserve">
         <v xml:space="preserve">
-                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque Ecoturístico que han sido mejor evaluados en este estado. 
- Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecoturístico que mejor calificación han recibido en Tabasco durante los últimos años. 
- Con esta prueba social como respaldo, hoy te daremos los Centro de Ecoturismo mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
+                    &lt;p&gt; ¿Estás buscando los mejores Parques Ecoturísticos en Tabasco? ¡Estás en el lugar correcto! Pues en este artículo vamos a presentarte cuáles son los  Parque de Ecoturismo que han sido mejor evaluados en este estado. 
+ Para esto, realizamos consultas en un montón de fuentes oficiales, redes sociales, rankings e incluso entrevistas para poder determinar cuáles son los  Parque Ecológico que mejor calificación han recibido en Tabasco durante los últimos años. 
+ Con esta prueba social como respaldo, hoy te daremos los Centro Ecoturístico mejor calificados y te compartiremos su ubicación, medios oficiales de contacto, horarios y cómo llegar hasta ellos, junto con la calificación promedio con la que cuenta cada lugar. 
  Así que prepárate y ¡a disfrutar del ecoturismo en Tabasco!&lt;/p&gt;                    
                     </v>
       </c>
       <c r="T3" t="str" xml:space="preserve">
         <v xml:space="preserve">
                     &lt;h2&gt;&lt;b&gt;Parque Ecoturístico Vivero Las Magnolias&lt;/b&gt;&lt;/h2&gt;
-                        &lt;p&gt;El Parque Ecoturístico undefined es una opción fantástica para tener una aventura natural en Tabasco. Su calificación promedio es de 4.7 respaldada por más de 106visitantes, así que no tenemos duda de que este lugar pertenece a la lista de los Parque Ecoturístico mejor rankeados de Tabasco y que se trata de uno de los principales atractivos naturales en la región. Así que ya sabes... ¿ganas de naturaleza?... pues el Parque Ecoturístico undefined es una grandísima opción.&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Parque Natural Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Para encontrar esta dirección, puedes usar un navegador como el waze o este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
-                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Centro Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los contactos disponibles del Parque Ecológico Vivero Las Magnolias son: &lt;/p&gt;
+                        &lt;p&gt;Bueno pues si eres de quienes ama estar en contacto con la naturaleza y andas por Tabasco, entonces no puedes perderte la experiencia de visitar el Parque Ecoturístico undefined. Con una calificación promedio de 4.7 estrellas de más de Excelente atención del joven y mucha variedad de plantas!!
+Compré tierra para macetas, me dijo el joven que era muy buena, pero huele muy mal, me pueden dar alguna sugerencia para eliminar ese olor tan fuerte?! Por favor!!,Me encantan todas las plantas, son muy amables, los precios justos🤩…,Muy bonito vivero visitantes, no tenemos duda de que se trata de un favorito de esta región. Así que nada...prepárate para sumergirte y disfrutar a tope de los paisajes naturales de Tabasco&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cómo llegar al Sitio Ecoturístico Vivero Las Magnolias? &lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;El Parque Ecoturístico se ubica enSauca 103, Jardines de Durango, 34200 Durango, Dgo.. Puedes ir a este lugar sin problemas manejando, sólo coloca su dirección oficial en waze, google maps o equivalente, o guíate con este &lt;a href='https://www.google.com.mx/maps/place/Vivero+Las+Magnolias/data=!4m7!3m6!1s0x869bb7b871872b85:0x65cc8cefdc6b7345!8m2!3d24.0374832!4d-104.6351623!16s%2Fg%2F11b6j5b_lw!19sChIJhSuHcbi3m4YRRXNr3O-MzGU?authuser=0&amp;hl=es&amp;rclk=1'&gt;Mapa del Parque Ecoturístico Vivero Las Magnolias&lt;/a&gt;&lt;/p&gt;
+                        &lt;h3&gt;&lt;b&gt;¿Cuáles son los contactos del Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los contactos disponibles del Parque Natural Vivero Las Magnolias son: &lt;/p&gt;
                             &lt;ul&gt;
                                 &lt;li&gt;&lt;b&gt;Teléfono:&lt;/b&gt;618 129 7673&lt;/li&gt;
                                 &lt;li&gt;&lt;b&gt;SitioWeb:&lt;/b&gt;web no disponible&lt;/li&gt;                                
                             &lt;/ul&gt;
-                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Ecoturístico Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
-                            &lt;p&gt;Los horarios oficiales del Centro Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
+                        &lt;h3&gt;&lt;b&gt;¿En qué horarios y días se puede visitar el Parque Natural Vivero Las Magnolias?&lt;/b&gt;&lt;/h3&gt;
+                            &lt;p&gt;Los horarios oficiales del Parque Ecoturístico Vivero Las Magnolias son los siguientes:&lt;/p&gt;                       
                             &lt;ul&gt;
                                 &lt;li&gt;Lunes de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Martes de 09:00 a 18:00&lt;/li&gt;
@@ -659,7 +660,7 @@
                                 &lt;li&gt;Sábado de 09:00 a 18:00&lt;/li&gt;
                                 &lt;li&gt;Domingo de 09:00 a 17:00&lt;/li&gt;
                             &lt;/ul&gt;
-                            &lt;p&gt;Aunque estos horarios están oficialmente vigentes, siempre es bueno consultar sus sitios de contacto y redes oficiales antes de visitarlos, por cualquier cambio extraordinario que pudieran tener.&lt;/p&gt;                 
+                            &lt;p&gt;A pesar de contar con horarios oficiales, te recomendamos siempre visitar sus sitios de contacto y redes oficiales antes de ir al lugar, así podrás identificar cualquier cambio extraordinario que hayan tenido.&lt;/p&gt;                 
                     </v>
       </c>
       <c r="U3" t="str" xml:space="preserve">

</xml_diff>